<commit_message>
(possibly) fixed seg fault/immediate finishing of event loop. Reduced number of reallocs for h_theData
</commit_message>
<xml_diff>
--- a/Results/Geant4_Performance_Results.xlsx
+++ b/Results/Geant4_Performance_Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>THREADS_PER_BLOCK</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>Feb-26-2:00pm</t>
+  </si>
+  <si>
+    <t>Mar-3-2:00pm</t>
+  </si>
+  <si>
+    <t>Updated caching code to reduce reallocs</t>
+  </si>
+  <si>
+    <t>Slowdown</t>
   </si>
 </sst>
 </file>
@@ -98,7 +107,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,6 +117,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -139,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -151,6 +166,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -430,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -446,12 +464,12 @@
     <col min="6" max="6" width="14.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="12.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="30.33203125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="1"/>
+    <col min="9" max="10" width="15.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="36.33203125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -480,40 +498,46 @@
         <v>12</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>500</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="5">
         <v>32</v>
       </c>
-      <c r="E2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="5">
         <v>50.93</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="5">
         <v>58.04</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="5">
         <v>7.08</v>
       </c>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="b">
         <v>0</v>
       </c>
@@ -541,41 +565,48 @@
       <c r="I3" s="3">
         <v>0</v>
       </c>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="J3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="5">
         <v>500</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="5">
         <v>32</v>
       </c>
-      <c r="E4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="E4" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="5">
         <v>34.159999999999997</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="5">
         <v>34.29</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="5">
         <v>0.06</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="5">
+        <f>G4/G3</f>
+        <v>2.4073291050035235</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="b">
         <v>0</v>
       </c>
@@ -603,60 +634,114 @@
       <c r="I5" s="3">
         <v>0.02</v>
       </c>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="J5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="5">
         <v>500</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>32</v>
       </c>
-      <c r="E6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="E6" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="5">
         <v>43.36</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="5">
         <v>43.39</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="5">
         <v>0.01</v>
       </c>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J6" s="5">
+        <f>G6/G5</f>
+        <v>3.2455089820359282</v>
+      </c>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3">
+        <v>500</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="1">
+        <v>13.47</v>
+      </c>
+      <c r="H7" s="1">
+        <v>13.56</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5">
+        <v>500</v>
+      </c>
+      <c r="D8" s="5">
+        <v>32</v>
+      </c>
+      <c r="E8" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="5">
+        <v>17.48</v>
+      </c>
+      <c r="H8" s="5">
+        <v>17.62</v>
+      </c>
+      <c r="I8" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J8" s="5">
+        <f>G8/G7</f>
+        <v>1.2976985894580548</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -667,6 +752,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>